<commit_message>
Added Score Mapping logic
</commit_message>
<xml_diff>
--- a/ai_tool_quality/modules/data/Questionnaire_Checklist.xlsx
+++ b/ai_tool_quality/modules/data/Questionnaire_Checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project_wissen\jacobs_aiops_project\qm_email_final\modules\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\008281\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524E47AA-CD86-4010-8C9E-FBCE502763DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B2E700-33DD-4C1D-95B6-6E8FDE512144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CFCE50ED-A835-4D9A-B1BD-66A4C38D0B72}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10360" xr2:uid="{CFCE50ED-A835-4D9A-B1BD-66A4C38D0B72}"/>
   </bookViews>
   <sheets>
     <sheet name="Contact type -Phone checklist" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="88">
   <si>
     <t>Contact type -Phone</t>
   </si>
@@ -355,6 +355,21 @@
   </si>
   <si>
     <t>No meaningful grammar mistakes</t>
+  </si>
+  <si>
+    <t>Score1</t>
+  </si>
+  <si>
+    <t>Score2</t>
+  </si>
+  <si>
+    <t>Score3</t>
+  </si>
+  <si>
+    <t>Score4</t>
+  </si>
+  <si>
+    <t>TScore</t>
   </si>
 </sst>
 </file>
@@ -482,7 +497,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -545,6 +560,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -910,27 +932,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{404E0E15-E478-4D6D-94A6-2EDFD8F1487F}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="111.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="12" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="20" customWidth="1"/>
+    <col min="1" max="1" width="6.54296875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="111.7265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" style="12" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="12.7265625" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.36328125" style="20" customWidth="1"/>
+    <col min="7" max="7" width="15.6328125" style="20" customWidth="1"/>
+    <col min="8" max="8" width="13" style="20" customWidth="1"/>
+    <col min="9" max="9" width="8.26953125" style="20" customWidth="1"/>
+    <col min="10" max="14" width="8.7265625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="5"/>
       <c r="B1" s="14" t="s">
         <v>0</v>
@@ -956,8 +978,23 @@
       <c r="I1" s="18" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J1" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -983,8 +1020,21 @@
         <v>50</v>
       </c>
       <c r="I2" s="19"/>
-    </row>
-    <row r="3" spans="1:9" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J2" s="19">
+        <v>2</v>
+      </c>
+      <c r="K2" s="19">
+        <v>0</v>
+      </c>
+      <c r="L2" s="19">
+        <v>2</v>
+      </c>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1010,8 +1060,21 @@
         <v>50</v>
       </c>
       <c r="I3" s="19"/>
-    </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J3" s="19">
+        <v>1</v>
+      </c>
+      <c r="K3" s="19">
+        <v>0</v>
+      </c>
+      <c r="L3" s="19">
+        <v>1</v>
+      </c>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1037,8 +1100,21 @@
         <v>50</v>
       </c>
       <c r="I4" s="19"/>
-    </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J4" s="19">
+        <v>1</v>
+      </c>
+      <c r="K4" s="19">
+        <v>0</v>
+      </c>
+      <c r="L4" s="19">
+        <v>1</v>
+      </c>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1062,8 +1138,19 @@
       </c>
       <c r="H5" s="11"/>
       <c r="I5" s="19"/>
-    </row>
-    <row r="6" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="J5" s="19">
+        <v>1</v>
+      </c>
+      <c r="K5" s="19">
+        <v>0</v>
+      </c>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1079,18 +1166,31 @@
       <c r="E6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="25" t="s">
         <v>54</v>
       </c>
       <c r="I6" s="19"/>
-    </row>
-    <row r="7" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="J6" s="19">
+        <v>0</v>
+      </c>
+      <c r="K6" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="L6" s="19">
+        <v>1</v>
+      </c>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1106,18 +1206,31 @@
       <c r="E7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="25" t="s">
         <v>57</v>
       </c>
       <c r="I7" s="19"/>
-    </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J7" s="19">
+        <v>0</v>
+      </c>
+      <c r="K7" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="L7" s="19">
+        <v>1</v>
+      </c>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1141,8 +1254,19 @@
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
-    </row>
-    <row r="9" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J8" s="19">
+        <v>1</v>
+      </c>
+      <c r="K8" s="19">
+        <v>0</v>
+      </c>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1166,8 +1290,19 @@
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
-    </row>
-    <row r="10" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J9" s="19">
+        <v>1</v>
+      </c>
+      <c r="K9" s="19">
+        <v>0</v>
+      </c>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1183,20 +1318,35 @@
       <c r="E10" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="H10" s="17" t="s">
+      <c r="H10" s="25" t="s">
         <v>61</v>
       </c>
       <c r="I10" s="17" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J10" s="19">
+        <v>0</v>
+      </c>
+      <c r="K10" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="L10" s="19">
+        <v>1</v>
+      </c>
+      <c r="M10" s="19">
+        <v>1</v>
+      </c>
+      <c r="N10" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1222,8 +1372,21 @@
         <v>63</v>
       </c>
       <c r="I11" s="19"/>
-    </row>
-    <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J11" s="19">
+        <v>0</v>
+      </c>
+      <c r="K11" s="19">
+        <v>1</v>
+      </c>
+      <c r="L11" s="19">
+        <v>2</v>
+      </c>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1249,8 +1412,21 @@
         <v>67</v>
       </c>
       <c r="I12" s="19"/>
-    </row>
-    <row r="13" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J12" s="19">
+        <v>0</v>
+      </c>
+      <c r="K12" s="19">
+        <v>1</v>
+      </c>
+      <c r="L12" s="19">
+        <v>2</v>
+      </c>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1272,8 +1448,21 @@
         <v>70</v>
       </c>
       <c r="I13" s="19"/>
-    </row>
-    <row r="14" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J13" s="19">
+        <v>1</v>
+      </c>
+      <c r="K13" s="19">
+        <v>2</v>
+      </c>
+      <c r="L13" s="19">
+        <v>3</v>
+      </c>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="42.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1295,8 +1484,21 @@
         <v>72</v>
       </c>
       <c r="I14" s="19"/>
-    </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J14" s="19">
+        <v>0</v>
+      </c>
+      <c r="K14" s="19">
+        <v>1</v>
+      </c>
+      <c r="L14" s="19">
+        <v>2</v>
+      </c>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1320,8 +1522,21 @@
         <v>50</v>
       </c>
       <c r="I15" s="19"/>
-    </row>
-    <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J15" s="19">
+        <v>2</v>
+      </c>
+      <c r="K15" s="19">
+        <v>0</v>
+      </c>
+      <c r="L15" s="19">
+        <v>2</v>
+      </c>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1343,8 +1558,19 @@
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="19"/>
-    </row>
-    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J16" s="19">
+        <v>1</v>
+      </c>
+      <c r="K16" s="19">
+        <v>0</v>
+      </c>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1368,8 +1594,19 @@
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="19"/>
-    </row>
-    <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J17" s="19">
+        <v>1</v>
+      </c>
+      <c r="K17" s="19">
+        <v>0</v>
+      </c>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1393,8 +1630,21 @@
         <v>50</v>
       </c>
       <c r="I18" s="19"/>
-    </row>
-    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J18" s="19">
+        <v>1</v>
+      </c>
+      <c r="K18" s="19">
+        <v>0</v>
+      </c>
+      <c r="L18" s="19">
+        <v>1</v>
+      </c>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1418,8 +1668,21 @@
         <v>50</v>
       </c>
       <c r="I19" s="19"/>
-    </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J19" s="19">
+        <v>1</v>
+      </c>
+      <c r="K19" s="19">
+        <v>0</v>
+      </c>
+      <c r="L19" s="19">
+        <v>1</v>
+      </c>
+      <c r="M19" s="19"/>
+      <c r="N19" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1441,8 +1704,21 @@
         <v>50</v>
       </c>
       <c r="I20" s="19"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="19">
+        <v>1</v>
+      </c>
+      <c r="K20" s="19">
+        <v>0</v>
+      </c>
+      <c r="L20" s="19">
+        <v>1</v>
+      </c>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -1462,8 +1738,19 @@
       </c>
       <c r="H21" s="11"/>
       <c r="I21" s="19"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="19">
+        <v>1</v>
+      </c>
+      <c r="K21" s="19">
+        <v>0</v>
+      </c>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1483,8 +1770,19 @@
       </c>
       <c r="H22" s="11"/>
       <c r="I22" s="19"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="19">
+        <v>1</v>
+      </c>
+      <c r="K22" s="19">
+        <v>0</v>
+      </c>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -1504,8 +1802,19 @@
       </c>
       <c r="H23" s="11"/>
       <c r="I23" s="19"/>
-    </row>
-    <row r="24" spans="1:9" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J23" s="19">
+        <v>1</v>
+      </c>
+      <c r="K23" s="19">
+        <v>0</v>
+      </c>
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="54.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -1525,8 +1834,19 @@
       </c>
       <c r="H24" s="19"/>
       <c r="I24" s="19"/>
-    </row>
-    <row r="25" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J24" s="19">
+        <v>1</v>
+      </c>
+      <c r="K24" s="19">
+        <v>0</v>
+      </c>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -1548,6 +1868,19 @@
         <v>50</v>
       </c>
       <c r="I25" s="19"/>
+      <c r="J25" s="19">
+        <v>3</v>
+      </c>
+      <c r="K25" s="19">
+        <v>0</v>
+      </c>
+      <c r="L25" s="19">
+        <v>3</v>
+      </c>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F6:H7">
@@ -1578,26 +1911,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE63AAD4-4036-4DCE-8CBB-AC0FD93F0DBF}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:I25"/>
+    <sheetView topLeftCell="B11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="106.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="44.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34" style="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="106.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" style="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" style="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" style="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.453125" style="24" customWidth="1"/>
+    <col min="7" max="7" width="20.54296875" style="24" customWidth="1"/>
+    <col min="8" max="8" width="19" style="24" customWidth="1"/>
+    <col min="9" max="9" width="10.26953125" style="24" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="8.7265625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="5"/>
       <c r="B1" s="21" t="s">
         <v>21</v>
@@ -1623,8 +1956,23 @@
       <c r="I1" s="18" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J1" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1650,8 +1998,21 @@
         <v>50</v>
       </c>
       <c r="I2" s="23"/>
-    </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J2" s="19">
+        <v>1</v>
+      </c>
+      <c r="K2" s="19">
+        <v>0</v>
+      </c>
+      <c r="L2" s="19">
+        <v>1</v>
+      </c>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1677,8 +2038,21 @@
         <v>50</v>
       </c>
       <c r="I3" s="23"/>
-    </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J3" s="19">
+        <v>1</v>
+      </c>
+      <c r="K3" s="19">
+        <v>0</v>
+      </c>
+      <c r="L3" s="19">
+        <v>1</v>
+      </c>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1702,8 +2076,19 @@
       </c>
       <c r="H4" s="11"/>
       <c r="I4" s="23"/>
-    </row>
-    <row r="5" spans="1:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J4" s="19">
+        <v>1</v>
+      </c>
+      <c r="K4" s="19">
+        <v>0</v>
+      </c>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="83.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1729,8 +2114,21 @@
         <v>54</v>
       </c>
       <c r="I5" s="23"/>
-    </row>
-    <row r="6" spans="1:9" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J5" s="19">
+        <v>0</v>
+      </c>
+      <c r="K5" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="L5" s="19">
+        <v>1</v>
+      </c>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1746,18 +2144,31 @@
       <c r="E6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="25" t="s">
         <v>57</v>
       </c>
       <c r="I6" s="23"/>
-    </row>
-    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J6" s="19">
+        <v>0</v>
+      </c>
+      <c r="K6" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="L6" s="19">
+        <v>1</v>
+      </c>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1773,20 +2184,35 @@
       <c r="E7" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="H7" s="23" t="s">
+      <c r="H7" s="26" t="s">
         <v>79</v>
       </c>
       <c r="I7" s="23" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J7" s="19">
+        <v>0</v>
+      </c>
+      <c r="K7" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="L7" s="19">
+        <v>1</v>
+      </c>
+      <c r="M7" s="19">
+        <v>1</v>
+      </c>
+      <c r="N7" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1802,20 +2228,35 @@
       <c r="E8" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="H8" s="23" t="s">
+      <c r="H8" s="26" t="s">
         <v>82</v>
       </c>
       <c r="I8" s="23" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J8" s="19">
+        <v>0</v>
+      </c>
+      <c r="K8" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="L8" s="19">
+        <v>1</v>
+      </c>
+      <c r="M8" s="19">
+        <v>1</v>
+      </c>
+      <c r="N8" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1841,8 +2282,21 @@
         <v>67</v>
       </c>
       <c r="I9" s="23"/>
-    </row>
-    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J9" s="19">
+        <v>0</v>
+      </c>
+      <c r="K9" s="19">
+        <v>1</v>
+      </c>
+      <c r="L9" s="19">
+        <v>2</v>
+      </c>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1868,8 +2322,21 @@
         <v>63</v>
       </c>
       <c r="I10" s="23"/>
-    </row>
-    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J10" s="19">
+        <v>0</v>
+      </c>
+      <c r="K10" s="19">
+        <v>1</v>
+      </c>
+      <c r="L10" s="19">
+        <v>2</v>
+      </c>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1885,20 +2352,35 @@
       <c r="E11" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="G11" s="23" t="s">
+      <c r="G11" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="H11" s="23" t="s">
+      <c r="H11" s="26" t="s">
         <v>61</v>
       </c>
       <c r="I11" s="23" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J11" s="19">
+        <v>0</v>
+      </c>
+      <c r="K11" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="L11" s="19">
+        <v>1</v>
+      </c>
+      <c r="M11" s="19">
+        <v>1</v>
+      </c>
+      <c r="N11" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1924,8 +2406,21 @@
         <v>50</v>
       </c>
       <c r="I12" s="23"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="19">
+        <v>1</v>
+      </c>
+      <c r="K12" s="19">
+        <v>0</v>
+      </c>
+      <c r="L12" s="19">
+        <v>1</v>
+      </c>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1947,8 +2442,21 @@
         <v>70</v>
       </c>
       <c r="I13" s="23"/>
-    </row>
-    <row r="14" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="J13" s="19">
+        <v>1</v>
+      </c>
+      <c r="K13" s="19">
+        <v>2</v>
+      </c>
+      <c r="L13" s="19">
+        <v>3</v>
+      </c>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1970,8 +2478,21 @@
         <v>72</v>
       </c>
       <c r="I14" s="23"/>
-    </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J14" s="19">
+        <v>0</v>
+      </c>
+      <c r="K14" s="19">
+        <v>1</v>
+      </c>
+      <c r="L14" s="19">
+        <v>2</v>
+      </c>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1995,8 +2516,21 @@
         <v>50</v>
       </c>
       <c r="I15" s="23"/>
-    </row>
-    <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J15" s="19">
+        <v>1</v>
+      </c>
+      <c r="K15" s="19">
+        <v>0</v>
+      </c>
+      <c r="L15" s="19">
+        <v>1</v>
+      </c>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2018,8 +2552,19 @@
       </c>
       <c r="H16" s="23"/>
       <c r="I16" s="23"/>
-    </row>
-    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J16" s="19">
+        <v>1</v>
+      </c>
+      <c r="K16" s="19">
+        <v>0</v>
+      </c>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2043,8 +2588,19 @@
       </c>
       <c r="H17" s="23"/>
       <c r="I17" s="23"/>
-    </row>
-    <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J17" s="19">
+        <v>1</v>
+      </c>
+      <c r="K17" s="19">
+        <v>0</v>
+      </c>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2068,8 +2624,21 @@
         <v>50</v>
       </c>
       <c r="I18" s="23"/>
-    </row>
-    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J18" s="19">
+        <v>1</v>
+      </c>
+      <c r="K18" s="19">
+        <v>0</v>
+      </c>
+      <c r="L18" s="19">
+        <v>1</v>
+      </c>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2093,8 +2662,21 @@
         <v>50</v>
       </c>
       <c r="I19" s="23"/>
-    </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J19" s="19">
+        <v>1</v>
+      </c>
+      <c r="K19" s="19">
+        <v>0</v>
+      </c>
+      <c r="L19" s="19">
+        <v>1</v>
+      </c>
+      <c r="M19" s="19"/>
+      <c r="N19" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2116,8 +2698,21 @@
         <v>50</v>
       </c>
       <c r="I20" s="23"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="19">
+        <v>1</v>
+      </c>
+      <c r="K20" s="19">
+        <v>0</v>
+      </c>
+      <c r="L20" s="19">
+        <v>1</v>
+      </c>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2137,8 +2732,19 @@
       </c>
       <c r="H21" s="11"/>
       <c r="I21" s="19"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="19">
+        <v>1</v>
+      </c>
+      <c r="K21" s="19">
+        <v>0</v>
+      </c>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2158,8 +2764,19 @@
       </c>
       <c r="H22" s="11"/>
       <c r="I22" s="19"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="19">
+        <v>1</v>
+      </c>
+      <c r="K22" s="19">
+        <v>0</v>
+      </c>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2179,8 +2796,19 @@
       </c>
       <c r="H23" s="11"/>
       <c r="I23" s="19"/>
-    </row>
-    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J23" s="19">
+        <v>1</v>
+      </c>
+      <c r="K23" s="19">
+        <v>0</v>
+      </c>
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -2200,8 +2828,19 @@
       </c>
       <c r="H24" s="23"/>
       <c r="I24" s="23"/>
-    </row>
-    <row r="25" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J24" s="19">
+        <v>1</v>
+      </c>
+      <c r="K24" s="19">
+        <v>0</v>
+      </c>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -2223,6 +2862,19 @@
         <v>50</v>
       </c>
       <c r="I25" s="23"/>
+      <c r="J25" s="19">
+        <v>3</v>
+      </c>
+      <c r="K25" s="19">
+        <v>0</v>
+      </c>
+      <c r="L25" s="19">
+        <v>3</v>
+      </c>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F5:H6">
@@ -2244,27 +2896,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED1313ED-377E-4259-9202-577B20A78EE4}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="86.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="1"/>
+    <col min="2" max="2" width="86.81640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="34" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="14.54296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.26953125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.26953125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1796875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1796875" style="1"/>
+    <col min="10" max="14" width="9.1796875" style="12"/>
+    <col min="15" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B1" s="7" t="s">
         <v>33</v>
       </c>
@@ -2289,8 +2942,23 @@
       <c r="I1" s="18" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J1" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -2316,8 +2984,21 @@
         <v>50</v>
       </c>
       <c r="I2" s="4"/>
-    </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J2" s="19">
+        <v>1</v>
+      </c>
+      <c r="K2" s="19">
+        <v>0</v>
+      </c>
+      <c r="L2" s="19">
+        <v>1</v>
+      </c>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -2343,8 +3024,21 @@
         <v>50</v>
       </c>
       <c r="I3" s="4"/>
-    </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J3" s="19">
+        <v>1</v>
+      </c>
+      <c r="K3" s="19">
+        <v>0</v>
+      </c>
+      <c r="L3" s="19">
+        <v>1</v>
+      </c>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -2368,8 +3062,19 @@
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="1:9" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J4" s="19">
+        <v>1</v>
+      </c>
+      <c r="K4" s="19">
+        <v>0</v>
+      </c>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="73" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -2385,18 +3090,31 @@
       <c r="E5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="25" t="s">
         <v>54</v>
       </c>
       <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J5" s="19">
+        <v>0</v>
+      </c>
+      <c r="K5" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="L5" s="19">
+        <v>1</v>
+      </c>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="73" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -2412,18 +3130,31 @@
       <c r="E6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="25" t="s">
         <v>57</v>
       </c>
       <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J6" s="19">
+        <v>0</v>
+      </c>
+      <c r="K6" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="L6" s="19">
+        <v>1</v>
+      </c>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -2449,8 +3180,21 @@
         <v>50</v>
       </c>
       <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J7" s="19">
+        <v>0</v>
+      </c>
+      <c r="K7" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="L7" s="19">
+        <v>1</v>
+      </c>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -2466,20 +3210,35 @@
       <c r="E8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="H8" s="23" t="s">
+      <c r="H8" s="26" t="s">
         <v>79</v>
       </c>
       <c r="I8" s="23" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="19">
+        <v>0</v>
+      </c>
+      <c r="K8" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="L8" s="19">
+        <v>1</v>
+      </c>
+      <c r="M8" s="19">
+        <v>1</v>
+      </c>
+      <c r="N8" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -2491,18 +3250,31 @@
       </c>
       <c r="D9" s="23"/>
       <c r="E9" s="23"/>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="H9" s="11" t="s">
         <v>70</v>
       </c>
       <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="J9" s="19">
+        <v>1</v>
+      </c>
+      <c r="K9" s="19">
+        <v>2</v>
+      </c>
+      <c r="L9" s="19">
+        <v>3</v>
+      </c>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -2524,8 +3296,21 @@
         <v>72</v>
       </c>
       <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J10" s="19">
+        <v>0</v>
+      </c>
+      <c r="K10" s="19">
+        <v>1</v>
+      </c>
+      <c r="L10" s="19">
+        <v>2</v>
+      </c>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -2549,8 +3334,21 @@
         <v>50</v>
       </c>
       <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J11" s="19">
+        <v>2</v>
+      </c>
+      <c r="K11" s="19">
+        <v>0</v>
+      </c>
+      <c r="L11" s="19">
+        <v>2</v>
+      </c>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -2572,8 +3370,19 @@
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J12" s="19">
+        <v>1</v>
+      </c>
+      <c r="K12" s="19">
+        <v>0</v>
+      </c>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -2597,8 +3406,19 @@
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J13" s="19">
+        <v>1</v>
+      </c>
+      <c r="K13" s="19">
+        <v>0</v>
+      </c>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="8">
         <v>13</v>
       </c>
@@ -2622,8 +3442,21 @@
         <v>50</v>
       </c>
       <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J14" s="19">
+        <v>1</v>
+      </c>
+      <c r="K14" s="19">
+        <v>0</v>
+      </c>
+      <c r="L14" s="19">
+        <v>1</v>
+      </c>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="9">
         <v>14</v>
       </c>
@@ -2647,8 +3480,21 @@
         <v>50</v>
       </c>
       <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J15" s="19">
+        <v>1</v>
+      </c>
+      <c r="K15" s="19">
+        <v>0</v>
+      </c>
+      <c r="L15" s="19">
+        <v>1</v>
+      </c>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="8">
         <v>15</v>
       </c>
@@ -2670,8 +3516,21 @@
         <v>50</v>
       </c>
       <c r="I16" s="4"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="19">
+        <v>1</v>
+      </c>
+      <c r="K16" s="19">
+        <v>0</v>
+      </c>
+      <c r="L16" s="19">
+        <v>1</v>
+      </c>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="8">
         <v>16</v>
       </c>
@@ -2691,8 +3550,19 @@
       </c>
       <c r="H17" s="11"/>
       <c r="I17" s="19"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="19">
+        <v>1</v>
+      </c>
+      <c r="K17" s="19">
+        <v>0</v>
+      </c>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="9">
         <v>17</v>
       </c>
@@ -2712,8 +3582,19 @@
       </c>
       <c r="H18" s="11"/>
       <c r="I18" s="19"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="19">
+        <v>1</v>
+      </c>
+      <c r="K18" s="19">
+        <v>0</v>
+      </c>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="8">
         <v>18</v>
       </c>
@@ -2733,8 +3614,19 @@
       </c>
       <c r="H19" s="11"/>
       <c r="I19" s="19"/>
-    </row>
-    <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J19" s="19">
+        <v>1</v>
+      </c>
+      <c r="K19" s="19">
+        <v>0</v>
+      </c>
+      <c r="L19" s="19"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A20" s="9">
         <v>19</v>
       </c>
@@ -2754,8 +3646,19 @@
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
-    </row>
-    <row r="21" spans="1:9" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J20" s="19">
+        <v>1</v>
+      </c>
+      <c r="K20" s="19">
+        <v>0</v>
+      </c>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="8">
         <v>20</v>
       </c>
@@ -2777,6 +3680,19 @@
         <v>50</v>
       </c>
       <c r="I21" s="4"/>
+      <c r="J21" s="19">
+        <v>3</v>
+      </c>
+      <c r="K21" s="19">
+        <v>0</v>
+      </c>
+      <c r="L21" s="19">
+        <v>3</v>
+      </c>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F5:H6">
@@ -2802,13 +3718,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -2816,7 +3732,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -2837,12 +3753,12 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -2850,7 +3766,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -2874,12 +3790,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -2887,7 +3803,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>38</v>
       </c>

</xml_diff>